<commit_message>
round 1 final entries
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/R1 Advanced.xlsx
+++ b/public/res/leaderboards/R1 Advanced.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamzaqureshi/Documents/Programming/Python/poker-tournament-leaderboard/public/res/leaderboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BCE776-F779-FD46-BD70-B5FFBB1DF20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A37F41-2A4C-9241-98FB-F87F3D78D199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$46</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
   <si>
     <t>Hamza Qureshi</t>
   </si>
@@ -167,6 +170,9 @@
   </si>
   <si>
     <t>Svarnim Agarwal</t>
+  </si>
+  <si>
+    <t>Jordan Hansen</t>
   </si>
 </sst>
 </file>
@@ -1015,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="139" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1324,14 +1330,8 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
+      <c r="B22" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1339,7 +1339,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
         <v>44</v>
@@ -1353,7 +1353,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
         <v>44</v>
@@ -1367,7 +1367,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
         <v>44</v>
@@ -1381,7 +1381,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
         <v>44</v>
@@ -1395,7 +1395,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
         <v>44</v>
@@ -1409,7 +1409,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
         <v>44</v>
@@ -1423,7 +1423,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
         <v>44</v>
@@ -1437,7 +1437,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
         <v>44</v>
@@ -1451,7 +1451,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
         <v>44</v>
@@ -1465,7 +1465,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
         <v>44</v>
@@ -1479,7 +1479,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
@@ -1493,7 +1493,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
         <v>44</v>
@@ -1507,7 +1507,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
         <v>44</v>
@@ -1521,7 +1521,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
@@ -1535,7 +1535,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
         <v>44</v>
@@ -1549,7 +1549,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
         <v>44</v>
@@ -1563,7 +1563,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
@@ -1577,7 +1577,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
         <v>44</v>
@@ -1591,7 +1591,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
         <v>44</v>
@@ -1605,7 +1605,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
         <v>44</v>
@@ -1619,7 +1619,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
         <v>44</v>
@@ -1633,7 +1633,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C44" t="s">
         <v>44</v>
@@ -1647,16 +1647,35 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45">
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D46" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D46">
+      <sortCondition ref="B1:B46"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>